<commit_message>
comm1 git commit -m comm1
</commit_message>
<xml_diff>
--- a/Utils/data.xlsx
+++ b/Utils/data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashpatel\eclipse-workspace\ExitTest\Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA515D0-4235-4F9D-BB5F-308BCAB9C531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDED5B35-AC30-4E31-8195-A4903AB7BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="779" activeTab="1" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="779" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
   </bookViews>
   <sheets>
-    <sheet name="LogInPageData" sheetId="1" r:id="rId1"/>
-    <sheet name="HomePageData" sheetId="2" r:id="rId2"/>
-    <sheet name="AddToCartPageData" sheetId="3" r:id="rId3"/>
-    <sheet name="LogoutPageData" sheetId="6" r:id="rId4"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="HomeData" sheetId="2" r:id="rId2"/>
+    <sheet name="AddToCartData" sheetId="3" r:id="rId3"/>
+    <sheet name="LogoutData" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -54,18 +54,9 @@
     <t>Password</t>
   </si>
   <si>
-    <t>whenUserEntersValidMobileNumberAndValidPassword</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
-    <t>whenUserEntersValidMobileNumberAndInvalidPassword</t>
-  </si>
-  <si>
-    <t>whenUserEntersInvalidMobileNumberAndValidPassword</t>
-  </si>
-  <si>
     <t>ProductSearch</t>
   </si>
   <si>
@@ -78,75 +69,36 @@
     <t>Your username or password is incorrect</t>
   </si>
   <si>
-    <t>whenUserWishlistProduct</t>
-  </si>
-  <si>
     <t>My Wishlist (1)</t>
   </si>
   <si>
-    <t>whenUserRemoveProductFromWishlist</t>
-  </si>
-  <si>
     <t>Empty Wishlist</t>
   </si>
   <si>
-    <t>whenUserClickOrders</t>
-  </si>
-  <si>
     <t>Flipkart.com: Your Order History</t>
   </si>
   <si>
-    <t>whenUserClickSuperCoins</t>
-  </si>
-  <si>
     <t>Flipkart SuperCoins – Re-usable rewards awarded by Flipkart on every Order! | Flipkart.com</t>
   </si>
   <si>
-    <t>whenUserClickFlipkartLogo</t>
-  </si>
-  <si>
-    <t>whenUserClickFlipkartPlusZone</t>
-  </si>
-  <si>
     <t>Flipkart Plus – The Ultimate Rewards Program for Flipkart Customers | Flipkart.com</t>
   </si>
   <si>
-    <t>whenUserClickCoupons</t>
-  </si>
-  <si>
-    <t>whenUserClickNotifications</t>
-  </si>
-  <si>
-    <t>whenUserAddsProductToCart</t>
-  </si>
-  <si>
     <t>Shopping Cart | Flipkart.com</t>
   </si>
   <si>
-    <t>whenUserRemoveProductFromCart</t>
-  </si>
-  <si>
     <t>Your cart is empty!</t>
   </si>
   <si>
-    <t>whenUserClickSaveForLater</t>
-  </si>
-  <si>
     <t>Saved For Later (1)</t>
   </si>
   <si>
-    <t>whenUserClickLogoutButton</t>
-  </si>
-  <si>
     <t>Nike Sneakers</t>
   </si>
   <si>
     <t>NIKE</t>
   </si>
   <si>
-    <t>whenUserClicksOnCheckSize</t>
-  </si>
-  <si>
     <t>Size Chart</t>
   </si>
   <si>
@@ -159,18 +111,9 @@
     <t>gibberish</t>
   </si>
   <si>
-    <t>whenUserClicksNIKE</t>
-  </si>
-  <si>
     <t>Assertion done on Expected Title</t>
   </si>
   <si>
-    <t>whenUserEntersInvalidMobileNumberAndInvalidPassword</t>
-  </si>
-  <si>
-    <t>whenUserSearchTheProduct</t>
-  </si>
-  <si>
     <t>94769352221</t>
   </si>
   <si>
@@ -180,10 +123,67 @@
     <t>All Notifications</t>
   </si>
   <si>
-    <t>whenUserClicksNextButton</t>
-  </si>
-  <si>
     <t>Showing 41 – 80 of 116 results for "Nike sneakers"</t>
+  </si>
+  <si>
+    <t>UserWishlistProduct</t>
+  </si>
+  <si>
+    <t>UserRemoveProductFromWishlist</t>
+  </si>
+  <si>
+    <t>UserClickOrders</t>
+  </si>
+  <si>
+    <t>UserClickSuperCoins</t>
+  </si>
+  <si>
+    <t>UserClickFlipkartLogo</t>
+  </si>
+  <si>
+    <t>UserClickFlipkartPlusZone</t>
+  </si>
+  <si>
+    <t>UserClickCoupons</t>
+  </si>
+  <si>
+    <t>UserClickNotifications</t>
+  </si>
+  <si>
+    <t>UserClicksNIKE</t>
+  </si>
+  <si>
+    <t>UserClicksNextButton</t>
+  </si>
+  <si>
+    <t>UserSearchTheProduct</t>
+  </si>
+  <si>
+    <t>UserEntersValidMobileNumberAndValidPassword</t>
+  </si>
+  <si>
+    <t>UserEntersInvalidMobileNumberAndValidPassword</t>
+  </si>
+  <si>
+    <t>UserEntersValidMobileNumberAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>UserEntersInvalidMobileNumberAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>UserAddsProductToCart</t>
+  </si>
+  <si>
+    <t>UserRemoveProductFromCart</t>
+  </si>
+  <si>
+    <t>UserClickSaveForLater</t>
+  </si>
+  <si>
+    <t>UserClicksOnCheckSize</t>
+  </si>
+  <si>
+    <t>UserClickLogoutButton</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866CE2D-7A03-41E5-A66E-D2508063588E}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -605,24 +605,24 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -630,62 +630,62 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25E9733-A6D2-4AA4-B618-C720A2BD77C8}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,10 +738,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -759,279 +759,279 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,94 +1071,94 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -1217,19 +1217,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>

</xml_diff>